<commit_message>
Fix Excel save for Streamlit cloud
</commit_message>
<xml_diff>
--- a/test6.xlsx
+++ b/test6.xlsx
@@ -596,7 +596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2302,6 +2302,67 @@
       </c>
       <c r="N27" s="3" t="n"/>
       <c r="O27" s="3" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>2025-11-21 14:16:06</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>SA01</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>Mixing Block</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="inlineStr">
+        <is>
+          <t>H1</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>Inner</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="n">
+        <v>111</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>FAIL</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="n"/>
+      <c r="O28" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>